<commit_message>
Builds oddb_calc.xml. Many missing formats
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -14,14 +14,14 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$6</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Sheet1!$3:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$11644</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$11633</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -83,40 +83,46 @@
     <t>Anwendungsgebiet Dosisstärke</t>
   </si>
   <si>
+    <t>nam</t>
+  </si>
+  <si>
+    <t>AstraZeneca AG</t>
+  </si>
+  <si>
+    <t>01.02.2.</t>
+  </si>
+  <si>
+    <t>N01BB09</t>
+  </si>
+  <si>
+    <t>Synthetika human</t>
+  </si>
+  <si>
+    <t>1 x 5 x 100</t>
+  </si>
+  <si>
+    <t>,.</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>ropivacainum</t>
+  </si>
+  <si>
+    <t>ropivacaini hydrochloridum 2 mg, natrii chloridum, aqua ad iniectabilia q.s. ad solutionem pro 1 ml.</t>
+  </si>
+  <si>
+    <t>Lokalanästhetikum</t>
+  </si>
+  <si>
     <t>Naropin 0,2 %, Infusionslösung / Injektionslösung</t>
   </si>
   <si>
-    <t>AstraZeneca AG</t>
-  </si>
-  <si>
-    <t>01.02.2.</t>
-  </si>
-  <si>
-    <t>N01BB09</t>
-  </si>
-  <si>
-    <t>Synthetika human</t>
-  </si>
-  <si>
-    <t>1 x 5 x 100</t>
+    <t>1 x 5 x 200</t>
   </si>
   <si>
     <t>ml</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>ropivacainum</t>
-  </si>
-  <si>
-    <t>ropivacaini hydrochloridum 2 mg, natrii chloridum, aqua ad iniectabilia q.s. ad solutionem pro 1 ml.</t>
-  </si>
-  <si>
-    <t>Lokalanästhetikum</t>
-  </si>
-  <si>
-    <t>1 x 5 x 200</t>
   </si>
 </sst>
 </file>
@@ -129,7 +135,7 @@
     <numFmt numFmtId="166" formatCode="DD/MM/YY;@"/>
     <numFmt numFmtId="167" formatCode="000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -175,6 +181,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="ARIAL"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -225,7 +237,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -331,6 +343,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -395,10 +411,10 @@
   </sheetPr>
   <dimension ref="1:6"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A11630" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1559,7 +1575,7 @@
       <c r="K5" s="26" t="n">
         <v>100</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="27" t="s">
         <v>25</v>
       </c>
       <c r="M5" s="5" t="s">
@@ -1587,7 +1603,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>21</v>
@@ -1614,10 +1630,10 @@
         <v>119</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Fix some occurences of selling_units
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -12,20 +12,22 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Sheet1!$3:$4</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="89">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -172,9 +174,6 @@
     <t>D11AF</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -242,6 +241,61 @@
   </si>
   <si>
     <t>aktive Immunisierung gegen Influenza, ab dem vollendeten 6. Lebensmonat</t>
+  </si>
+  <si>
+    <t>Infloran, capsule</t>
+  </si>
+  <si>
+    <t>Desma Healthcare SpA, Torino succursale di Chiasso</t>
+  </si>
+  <si>
+    <t>04.09.0.</t>
+  </si>
+  <si>
+    <t>A07FA01</t>
+  </si>
+  <si>
+    <t>Bakterien- und Hefepräparate</t>
+  </si>
+  <si>
+    <t>2x10</t>
+  </si>
+  <si>
+    <t>Kapsel(n)</t>
+  </si>
+  <si>
+    <t>lactobacillus acidophilus cryodesiccatus, bifidobacterium infantis</t>
+  </si>
+  <si>
+    <t>lactobacillus acidophilus cryodesiccatus min. 10^9 CFU, bifidobacterium infantis min. 10^9 CFU, color.: E 127, E 132, E 104, excipiens pro capsula.</t>
+  </si>
+  <si>
+    <t>Normalizzazione della flora intestinale
+Trattamento sintomatico della diarrea</t>
+  </si>
+  <si>
+    <t>Kamillin Medipharm, Bad</t>
+  </si>
+  <si>
+    <t>10.08.0.</t>
+  </si>
+  <si>
+    <t>D03AX</t>
+  </si>
+  <si>
+    <t>Phytotherapeutika</t>
+  </si>
+  <si>
+    <t>25 x 40</t>
+  </si>
+  <si>
+    <t>matricariae extractum isopropanolicum liquidum</t>
+  </si>
+  <si>
+    <t>matricariae extractum isopropanolicum liquidum 98.9 g corresp. levomenolum 10-50 mg, ratio: 1:2-2.8, excipiens ad solutionem pro 100 g.</t>
+  </si>
+  <si>
+    <t>Bei Hauterkrankungen</t>
   </si>
 </sst>
 </file>
@@ -350,7 +404,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -473,6 +527,38 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -492,15 +578,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>108000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>994680</xdr:colOff>
+      <xdr:colOff>1021320</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>542160</xdr:rowOff>
+      <xdr:rowOff>541800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -513,8 +599,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="81000" y="0"/>
-          <a:ext cx="1780200" cy="542160"/>
+          <a:off x="108000" y="0"/>
+          <a:ext cx="1779840" cy="541800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -534,12 +620,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="P9" activeCellId="0" sqref="P9"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="12:12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -850,23 +936,23 @@
       <c r="K8" s="26" t="n">
         <v>11</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>48</v>
+      <c r="L8" s="1" t="n">
+        <v>43454</v>
       </c>
       <c r="M8" s="27" t="s">
         <v>43</v>
       </c>
       <c r="N8" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="O8" s="24" t="s">
+      <c r="P8" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="P8" s="24" t="s">
+      <c r="Q8" s="24" t="s">
         <v>51</v>
-      </c>
-      <c r="Q8" s="24" t="s">
-        <v>52</v>
       </c>
       <c r="R8" s="0"/>
     </row>
@@ -878,16 +964,16 @@
         <v>1</v>
       </c>
       <c r="C9" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>35</v>
@@ -905,22 +991,22 @@
         <v>19</v>
       </c>
       <c r="L9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M9" s="27" t="s">
         <v>57</v>
-      </c>
-      <c r="M9" s="27" t="s">
-        <v>58</v>
       </c>
       <c r="N9" s="28" t="s">
         <v>27</v>
       </c>
       <c r="O9" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="P9" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="P9" s="24" t="s">
+      <c r="Q9" s="24" t="s">
         <v>60</v>
-      </c>
-      <c r="Q9" s="24" t="s">
-        <v>61</v>
       </c>
       <c r="R9" s="0"/>
     </row>
@@ -932,19 +1018,19 @@
         <v>23</v>
       </c>
       <c r="C10" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="H10" s="25" t="n">
         <v>27661</v>
@@ -959,27 +1045,135 @@
         <v>10</v>
       </c>
       <c r="L10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M10" s="27" t="s">
         <v>67</v>
-      </c>
-      <c r="M10" s="27" t="s">
-        <v>68</v>
       </c>
       <c r="N10" s="28" t="s">
         <v>27</v>
       </c>
       <c r="O10" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="P10" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="P10" s="24" t="s">
+      <c r="Q10" s="24" t="s">
         <v>70</v>
-      </c>
-      <c r="Q10" s="24" t="s">
-        <v>71</v>
       </c>
       <c r="R10" s="0"/>
     </row>
+    <row r="11" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="31" t="n">
+        <v>679</v>
+      </c>
+      <c r="B11" s="32" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="34" t="n">
+        <v>28230</v>
+      </c>
+      <c r="I11" s="34" t="n">
+        <v>41599</v>
+      </c>
+      <c r="J11" s="34" t="n">
+        <v>43247</v>
+      </c>
+      <c r="K11" s="35" t="n">
+        <v>12</v>
+      </c>
+      <c r="L11" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="N11" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="P11" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q11" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="R11" s="0"/>
+    </row>
+    <row r="12" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="31" t="n">
+        <v>43454</v>
+      </c>
+      <c r="B12" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="34" t="n">
+        <v>29650</v>
+      </c>
+      <c r="I12" s="34" t="n">
+        <v>29650</v>
+      </c>
+      <c r="J12" s="34" t="n">
+        <v>43905</v>
+      </c>
+      <c r="K12" s="35" t="n">
+        <v>101</v>
+      </c>
+      <c r="L12" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="M12" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="N12" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="P12" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q12" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="R12" s="0"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A4:R7"/>
+  <autoFilter ref="A4:R11634"/>
   <mergeCells count="2">
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:D3"/>

</xml_diff>

<commit_message>
Added rule to fix selling_units for pkg_size like 1500 ml
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="97">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -296,6 +296,31 @@
   </si>
   <si>
     <t>Bei Hauterkrankungen</t>
+  </si>
+  <si>
+    <t>bicaNova 1,5 % Glucose, Peritonealdialyselösung</t>
+  </si>
+  <si>
+    <t>Fresenius Medical Care (Schweiz) AG</t>
+  </si>
+  <si>
+    <t>05.04.0.</t>
+  </si>
+  <si>
+    <t>B05DB</t>
+  </si>
+  <si>
+    <t>1500 ml</t>
+  </si>
+  <si>
+    <t>natrii chloridum, natrii hydrogenocarbonas, calcii chloridum dihydricum, magnesii chloridum hexahydricum, glucosum anhydricum, natrium, calcium, magnesium, chloridum, hydrogenocarbonas, glucosum</t>
+  </si>
+  <si>
+    <t>I) et II) corresp.: natrii chloridum 5.5 g, natrii hydrogenocarbonas 3.36 g, calcii chloridum dihydricum 184 mg, magnesii chloridum hexahydricum 102 mg, glucosum anhydricum 15 g ut glucosum monohydricum, aqua ad iniectabilia q.s. ad solutionem pro 1000 ml.
+Corresp. natrium 134 mmol, calcium 1.25 mmol, magnesium 0.5 mmol, chloridum 98.5 mmol, hydrogenocarbonas 39 mmol, glucosum 83.25 mmol.</t>
+  </si>
+  <si>
+    <t>Peritonealdialyse</t>
   </si>
 </sst>
 </file>
@@ -620,19 +645,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2355" topLeftCell="A5" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="12:12"/>
+      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="13:13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.00510204081633"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.28061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.8571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3877551020408"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="34.7091836734694"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.56632653061224"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.7091836734694"/>
@@ -1172,6 +1197,58 @@
       </c>
       <c r="R12" s="0"/>
     </row>
+    <row r="13" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="31" t="n">
+        <v>58277</v>
+      </c>
+      <c r="B13" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="34" t="n">
+        <v>39638</v>
+      </c>
+      <c r="I13" s="34" t="n">
+        <v>39638</v>
+      </c>
+      <c r="J13" s="34" t="n">
+        <v>43289</v>
+      </c>
+      <c r="K13" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="M13" s="0"/>
+      <c r="N13" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="P13" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q13" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="R13" s="0"/>
+    </row>
   </sheetData>
   <autoFilter ref="A4:R11634"/>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Corrected calculation for measure
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -321,6 +321,30 @@
   </si>
   <si>
     <t>Peritonealdialyse</t>
+  </si>
+  <si>
+    <t>Muse 125 ug, Urethrastab</t>
+  </si>
+  <si>
+    <t>MEDA Pharma GmbH</t>
+  </si>
+  <si>
+    <t>05.99.0.</t>
+  </si>
+  <si>
+    <t>G04BE01</t>
+  </si>
+  <si>
+    <t>6x1 Urethrastab</t>
+  </si>
+  <si>
+    <t>alprostadilum</t>
+  </si>
+  <si>
+    <t>alprostadilum 125 µg, excipiens ad gelatum pro praeparatione.</t>
+  </si>
+  <si>
+    <t>Erektile Dysfunktion</t>
   </si>
 </sst>
 </file>
@@ -645,12 +669,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2355" topLeftCell="A5" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="2355" topLeftCell="A4" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="13:13"/>
+      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="14:14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1249,6 +1273,58 @@
       </c>
       <c r="R13" s="0"/>
     </row>
+    <row r="14" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="31" t="n">
+        <v>54525</v>
+      </c>
+      <c r="B14" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="34" t="n">
+        <v>35852</v>
+      </c>
+      <c r="I14" s="34" t="n">
+        <v>35852</v>
+      </c>
+      <c r="J14" s="34" t="n">
+        <v>43553</v>
+      </c>
+      <c r="K14" s="35" t="n">
+        <v>36</v>
+      </c>
+      <c r="L14" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="M14" s="0"/>
+      <c r="N14" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="O14" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="P14" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q14" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="R14" s="0"/>
+    </row>
   </sheetData>
   <autoFilter ref="A4:R11634"/>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Fix Infusionsemulsion for Nutriflex
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -12,22 +12,24 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Sheet1!$3:$4</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="113">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -345,6 +347,35 @@
   </si>
   <si>
     <t>Erektile Dysfunktion</t>
+  </si>
+  <si>
+    <t>Nutriflex Lipid plus, Infusionsemulsion, 1250ml</t>
+  </si>
+  <si>
+    <t>B. Braun Medical AG</t>
+  </si>
+  <si>
+    <t>07.01.2.</t>
+  </si>
+  <si>
+    <t>B05BA10</t>
+  </si>
+  <si>
+    <t>5 x 1250</t>
+  </si>
+  <si>
+    <t>glucosum anhydricum, natrii dihydrogenophosphas dihydricus, zinci acetas dihydricus, isoleucinum, leucinum, lysinum anhydricum, methioninum, phenylalaninum, threoninum, tryptophanum, valinum, argininum, histidinum, alaninum, acidum asparticum, acidum glutamicum, glycinum, prolinum, serinum, natrii hydroxidum, natrii chloridum, natrii acetas trihydricus, kalii acetas, magnesii acetas tetrahydricus, calcii chloridum dihydricum, aminoacida, nitrogenia, carbohydrata, materia crassa, natrium, kalium, magnesium, calcium, zincum, chloridum, phosphas, acetas, sojae oleum, triglycerida saturata media</t>
+  </si>
+  <si>
+    <t>I) Glucoselösung: glucosum anhydricum 150 g ut glucosum monohydricum, natrii dihydrogenophosphas dihydricus 2.34 g, zinci acetas dihydricus 6.58 mg, aqua ad iniectabilia q.s. ad solutionem pro 500 ml.
+II) Fettemulsion: sojae oleum 25 g, triglycerida saturata media 25 g, lecithinum ex ovo, glycerolum, natrii oleas, aqua ad iniectabilia q.s. ad emulsionem pro 250 ml.
+III) Aminosäurenlösung: isoleucinum 2.82 g, leucinum 3.76 g, lysinum anhydricum 2.73 g ut lysinum monohydricum, methioninum 2.35 g, phenylalaninum 4.21 g, threoninum 2.18 g, tryptophanum 680 mg, valinum 3.12 g, argininum 3.24 g, histidinum 1.5 g ut histidini hydrochloridum monohydricum, alaninum 5.82 g, acidum asparticum 1.8 g, acidum glutamicum 4.21 g, glycinum 1.98 g, prolinum 4.08 g, serinum 3.6 g, natrii hydroxidum 0.976 g, natrii chloridum 0.503 g, natrii acetas trihydricus 0.277 g, kalii acetas 3.434 g, magnesii acetas tetrahydricus 0.858 g, calcii chloridum dihydricum 0.588 g, aqua ad iniectabilia q.s. ad solutionem pro 500 ml.
+.
+I) et II) et III) corresp.: aminoacida 38.4 g/l, nitrogenia 5.44 g/l, carbohydrata 120 g/l, materia crassa 40 g/l, natrium 40 mmol/l, kalium 28 mmol/l, magnesium 3.2 mmol/l, calcium 3.2 mmol/l, zincum 0.024 mmol/l, chloridum 36 mmol/l, phosphas 12 mmol/l, acetas 36 mmol/l, in emulsione recenter mixta 1000 ml.
+Corresp. 4240 kJ pro 1 l.</t>
+  </si>
+  <si>
+    <t>Parenterale Ernährung</t>
   </si>
 </sst>
 </file>
@@ -627,15 +658,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>108000</xdr:colOff>
+      <xdr:colOff>135000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1021320</xdr:colOff>
+      <xdr:colOff>1047960</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>541800</xdr:rowOff>
+      <xdr:rowOff>541440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -648,8 +679,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="108000" y="0"/>
-          <a:ext cx="1779840" cy="541800"/>
+          <a:off x="135000" y="0"/>
+          <a:ext cx="1779480" cy="541440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -669,12 +700,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2355" topLeftCell="A4" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="2070" topLeftCell="A4" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="14:14"/>
+      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="15:15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1113,220 +1144,271 @@
       </c>
       <c r="R10" s="0"/>
     </row>
-    <row r="11" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="31" t="n">
+    <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="23" t="n">
         <v>679</v>
       </c>
-      <c r="B11" s="32" t="n">
+      <c r="B11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="32" t="s">
+      <c r="G11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H11" s="34" t="n">
+      <c r="H11" s="25" t="n">
         <v>28230</v>
       </c>
-      <c r="I11" s="34" t="n">
+      <c r="I11" s="25" t="n">
         <v>41599</v>
       </c>
-      <c r="J11" s="34" t="n">
+      <c r="J11" s="25" t="n">
         <v>43247</v>
       </c>
-      <c r="K11" s="35" t="n">
+      <c r="K11" s="26" t="n">
         <v>12</v>
       </c>
-      <c r="L11" s="32" t="s">
+      <c r="L11" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="M11" s="36" t="s">
+      <c r="M11" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="N11" s="37" t="s">
+      <c r="N11" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="O11" s="33" t="s">
+      <c r="O11" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="P11" s="33" t="s">
+      <c r="P11" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="Q11" s="38" t="s">
+      <c r="Q11" s="29" t="s">
         <v>80</v>
       </c>
       <c r="R11" s="0"/>
     </row>
-    <row r="12" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="31" t="n">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="23" t="n">
         <v>43454</v>
       </c>
-      <c r="B12" s="32" t="n">
+      <c r="B12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G12" s="32" t="s">
+      <c r="G12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H12" s="34" t="n">
+      <c r="H12" s="25" t="n">
         <v>29650</v>
       </c>
-      <c r="I12" s="34" t="n">
+      <c r="I12" s="25" t="n">
         <v>29650</v>
       </c>
-      <c r="J12" s="34" t="n">
+      <c r="J12" s="25" t="n">
         <v>43905</v>
       </c>
-      <c r="K12" s="35" t="n">
+      <c r="K12" s="26" t="n">
         <v>101</v>
       </c>
-      <c r="L12" s="32" t="s">
+      <c r="L12" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="M12" s="36" t="s">
+      <c r="M12" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="N12" s="37" t="s">
+      <c r="N12" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="O12" s="33" t="s">
+      <c r="O12" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="P12" s="33" t="s">
+      <c r="P12" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="Q12" s="33" t="s">
+      <c r="Q12" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="R12" s="0"/>
     </row>
-    <row r="13" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="31" t="n">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="23" t="n">
         <v>58277</v>
       </c>
-      <c r="B13" s="32" t="n">
+      <c r="B13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G13" s="32" t="s">
+      <c r="G13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="34" t="n">
+      <c r="H13" s="25" t="n">
         <v>39638</v>
       </c>
-      <c r="I13" s="34" t="n">
+      <c r="I13" s="25" t="n">
         <v>39638</v>
       </c>
-      <c r="J13" s="34" t="n">
+      <c r="J13" s="25" t="n">
         <v>43289</v>
       </c>
-      <c r="K13" s="35" t="n">
+      <c r="K13" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="L13" s="32" t="s">
+      <c r="L13" s="1" t="s">
         <v>93</v>
       </c>
       <c r="M13" s="0"/>
-      <c r="N13" s="37" t="s">
+      <c r="N13" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="O13" s="33" t="s">
+      <c r="O13" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="P13" s="38" t="s">
+      <c r="P13" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="Q13" s="33" t="s">
+      <c r="Q13" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="R13" s="0"/>
     </row>
-    <row r="14" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="31" t="n">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="23" t="n">
         <v>54525</v>
       </c>
-      <c r="B14" s="32" t="n">
+      <c r="B14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="34" t="n">
+      <c r="H14" s="25" t="n">
         <v>35852</v>
       </c>
-      <c r="I14" s="34" t="n">
+      <c r="I14" s="25" t="n">
         <v>35852</v>
       </c>
-      <c r="J14" s="34" t="n">
+      <c r="J14" s="25" t="n">
         <v>43553</v>
       </c>
-      <c r="K14" s="35" t="n">
+      <c r="K14" s="26" t="n">
         <v>36</v>
       </c>
-      <c r="L14" s="32" t="s">
+      <c r="L14" s="1" t="s">
         <v>101</v>
       </c>
       <c r="M14" s="0"/>
-      <c r="N14" s="37" t="s">
+      <c r="N14" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="O14" s="33" t="s">
+      <c r="O14" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="P14" s="33" t="s">
+      <c r="P14" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="Q14" s="33" t="s">
+      <c r="Q14" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="R14" s="0"/>
+    </row>
+    <row r="15" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="31" t="n">
+        <v>55594</v>
+      </c>
+      <c r="B15" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="34" t="n">
+        <v>37172</v>
+      </c>
+      <c r="I15" s="34" t="n">
+        <v>37172</v>
+      </c>
+      <c r="J15" s="34" t="n">
+        <v>43863</v>
+      </c>
+      <c r="K15" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="M15" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="N15" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="P15" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q15" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="R15" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:R11634"/>
+  <autoFilter ref="A4:R7"/>
   <mergeCells count="2">
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:D3"/>

</xml_diff>

<commit_message>
Emit compositions for --calc
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="121">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -376,6 +376,30 @@
   </si>
   <si>
     <t>Parenterale Ernährung</t>
+  </si>
+  <si>
+    <t>Lapidar 4, Filmtabletten</t>
+  </si>
+  <si>
+    <t>Kräuterpfarrer Künzle AG</t>
+  </si>
+  <si>
+    <t>02.08.1.</t>
+  </si>
+  <si>
+    <t>C05CA51</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>rutosidum trihydricum, aescinum</t>
+  </si>
+  <si>
+    <t>rutosidum trihydricum 20 mg, aescinum 25 mg, aromatica, excipiens pro compresso.</t>
+  </si>
+  <si>
+    <t>Symptome bei Krampfadern</t>
   </si>
 </sst>
 </file>
@@ -700,12 +724,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2070" topLeftCell="A4" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="15:15"/>
+      <selection pane="bottomLeft" activeCell="A16" activeCellId="0" sqref="16:16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1407,6 +1431,60 @@
       </c>
       <c r="R15" s="0"/>
     </row>
+    <row r="16" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="31" t="n">
+        <v>10386</v>
+      </c>
+      <c r="B16" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="34" t="n">
+        <v>13027</v>
+      </c>
+      <c r="I16" s="34" t="n">
+        <v>13027</v>
+      </c>
+      <c r="J16" s="34" t="n">
+        <v>42358</v>
+      </c>
+      <c r="K16" s="35" t="n">
+        <v>47</v>
+      </c>
+      <c r="L16" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="M16" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="N16" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="O16" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="P16" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q16" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="R16" s="0"/>
+    </row>
   </sheetData>
   <autoFilter ref="A4:R7"/>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Remove unnecessary spaces from ARTICLE.NAME in oddb_calc.xml
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="129">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -400,6 +400,30 @@
   </si>
   <si>
     <t>Symptome bei Krampfadern</t>
+  </si>
+  <si>
+    <t>Magnesiumchlorid 0,5 molar B. Braun, Zusatzampulle für              Infusionslösungen</t>
+  </si>
+  <si>
+    <t>05.03.2.</t>
+  </si>
+  <si>
+    <t>B05XA11</t>
+  </si>
+  <si>
+    <t>5 x 10 mL</t>
+  </si>
+  <si>
+    <t>Ampulle(n)</t>
+  </si>
+  <si>
+    <t>magnesium, chloridum</t>
+  </si>
+  <si>
+    <t>magnesium 500 mmol, chloridum 1000 mmol, aqua ad iniectabilia q.s. ad solutionem pro 1000 ml.</t>
+  </si>
+  <si>
+    <t>Magnesiummangel</t>
   </si>
 </sst>
 </file>
@@ -724,12 +748,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2070" topLeftCell="A4" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A16" activeCellId="0" sqref="16:16"/>
+      <selection pane="bottomLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1485,6 +1509,60 @@
       </c>
       <c r="R16" s="0"/>
     </row>
+    <row r="17" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="31" t="n">
+        <v>45882</v>
+      </c>
+      <c r="B17" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="G17" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="34" t="n">
+        <v>31180</v>
+      </c>
+      <c r="I17" s="34" t="n">
+        <v>31180</v>
+      </c>
+      <c r="J17" s="34" t="n">
+        <v>43340</v>
+      </c>
+      <c r="K17" s="35" t="n">
+        <v>20</v>
+      </c>
+      <c r="L17" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="M17" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="N17" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="O17" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="P17" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q17" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="R17" s="0"/>
+    </row>
   </sheetData>
   <autoFilter ref="A4:R7"/>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Remove unnecessary spaces from ARTICLE.PKG_SIZE in oddb_calc.xml
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="136">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -424,6 +424,27 @@
   </si>
   <si>
     <t>Magnesiummangel</t>
+  </si>
+  <si>
+    <t>Lidocain 1% Streuli, Injektionslösung (Ampullen)</t>
+  </si>
+  <si>
+    <t>Streuli Pharma AG</t>
+  </si>
+  <si>
+    <t>N01BB02</t>
+  </si>
+  <si>
+    <t>10 x  2</t>
+  </si>
+  <si>
+    <t>lidocaini hydrochloridum</t>
+  </si>
+  <si>
+    <t>lidocaini hydrochloridum 10 mg, natrii chloridum, aqua ad iniectabilia q.s. ad solutionem pro 1 ml.</t>
+  </si>
+  <si>
+    <t>Lokalanaestheticum</t>
   </si>
 </sst>
 </file>
@@ -748,12 +769,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2070" topLeftCell="A4" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="18:18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1563,6 +1584,60 @@
       </c>
       <c r="R17" s="0"/>
     </row>
+    <row r="18" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="31" t="n">
+        <v>30015</v>
+      </c>
+      <c r="B18" s="32" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="34" t="n">
+        <v>23410</v>
+      </c>
+      <c r="I18" s="34" t="n">
+        <v>23410</v>
+      </c>
+      <c r="J18" s="34" t="n">
+        <v>43552</v>
+      </c>
+      <c r="K18" s="35" t="n">
+        <v>10</v>
+      </c>
+      <c r="L18" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="M18" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="N18" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="O18" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="P18" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q18" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="R18" s="0"/>
+    </row>
   </sheetData>
   <autoFilter ref="A4:R7"/>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Remove unnecessary spaces from ARTICLE.GALENIC_FORM in oddb_calc.xml
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="145">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -445,6 +445,34 @@
   </si>
   <si>
     <t>Lokalanaestheticum</t>
+  </si>
+  <si>
+    <t>Rocephin 500 mg i.v., Trockenampullen + Solvens</t>
+  </si>
+  <si>
+    <t>Roche Pharma (Schweiz) AG</t>
+  </si>
+  <si>
+    <t>08.01.3.</t>
+  </si>
+  <si>
+    <t>J01DD04</t>
+  </si>
+  <si>
+    <t>5 + 5</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>ceftriaxonum</t>
+  </si>
+  <si>
+    <t>Praeparatio sicca: ceftriaxonum 500 mg ut ceftriaxonum natricum pro vitro.
+Solvens: aqua ad iniectabilia 5 ml.</t>
+  </si>
+  <si>
+    <t>Infektionskrankheiten</t>
   </si>
 </sst>
 </file>
@@ -769,12 +797,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2070" topLeftCell="A4" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="18:18"/>
+      <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="19:19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1638,6 +1666,60 @@
       </c>
       <c r="R18" s="0"/>
     </row>
+    <row r="19" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="31" t="n">
+        <v>44625</v>
+      </c>
+      <c r="B19" s="32" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="34" t="n">
+        <v>30098</v>
+      </c>
+      <c r="I19" s="34" t="n">
+        <v>30098</v>
+      </c>
+      <c r="J19" s="34" t="n">
+        <v>42842</v>
+      </c>
+      <c r="K19" s="35" t="n">
+        <v>59</v>
+      </c>
+      <c r="L19" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="M19" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="N19" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="O19" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="P19" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q19" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="R19" s="0"/>
+    </row>
   </sheetData>
   <autoFilter ref="A4:R7"/>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Reorganized for easiear comparision with oddb.org
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -12,17 +12,19 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Sheet1!$3:$4</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -581,7 +583,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -704,38 +706,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -755,15 +725,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>135000</xdr:colOff>
+      <xdr:colOff>162000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1047960</xdr:colOff>
+      <xdr:colOff>1074600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>541440</xdr:rowOff>
+      <xdr:rowOff>541080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -776,8 +746,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="135000" y="0"/>
-          <a:ext cx="1779480" cy="541440"/>
+          <a:off x="162000" y="0"/>
+          <a:ext cx="1779120" cy="541080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -800,16 +770,16 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2070" topLeftCell="A4" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="1830" topLeftCell="A4" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="19:19"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.00510204081633"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.28061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.8877551020408"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="34.7091836734694"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.56632653061224"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.7091836734694"/>
@@ -1241,7 +1211,7 @@
       </c>
       <c r="R10" s="0"/>
     </row>
-    <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="n">
         <v>679</v>
       </c>
@@ -1293,7 +1263,6 @@
       <c r="Q11" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="R11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="n">
@@ -1450,278 +1419,274 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="31" t="n">
+    <row r="15" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="23" t="n">
         <v>55594</v>
       </c>
-      <c r="B15" s="32" t="n">
+      <c r="B15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F15" s="32" t="s">
+      <c r="F15" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="G15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="34" t="n">
+      <c r="H15" s="25" t="n">
         <v>37172</v>
       </c>
-      <c r="I15" s="34" t="n">
+      <c r="I15" s="25" t="n">
         <v>37172</v>
       </c>
-      <c r="J15" s="34" t="n">
+      <c r="J15" s="25" t="n">
         <v>43863</v>
       </c>
-      <c r="K15" s="35" t="n">
+      <c r="K15" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="L15" s="32" t="s">
+      <c r="L15" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="M15" s="36" t="s">
+      <c r="M15" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="N15" s="37" t="s">
+      <c r="N15" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="O15" s="33" t="s">
+      <c r="O15" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="P15" s="38" t="s">
+      <c r="P15" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="Q15" s="33" t="s">
+      <c r="Q15" s="24" t="s">
         <v>112</v>
       </c>
       <c r="R15" s="0"/>
     </row>
-    <row r="16" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="31" t="n">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="23" t="n">
         <v>10386</v>
       </c>
-      <c r="B16" s="32" t="n">
+      <c r="B16" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="G16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="34" t="n">
+      <c r="H16" s="25" t="n">
         <v>13027</v>
       </c>
-      <c r="I16" s="34" t="n">
+      <c r="I16" s="25" t="n">
         <v>13027</v>
       </c>
-      <c r="J16" s="34" t="n">
+      <c r="J16" s="25" t="n">
         <v>42358</v>
       </c>
-      <c r="K16" s="35" t="n">
+      <c r="K16" s="26" t="n">
         <v>47</v>
       </c>
-      <c r="L16" s="32" t="s">
+      <c r="L16" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="M16" s="36" t="s">
+      <c r="M16" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="N16" s="37" t="s">
+      <c r="N16" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="O16" s="33" t="s">
+      <c r="O16" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="P16" s="33" t="s">
+      <c r="P16" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="Q16" s="33" t="s">
+      <c r="Q16" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="R16" s="0"/>
     </row>
-    <row r="17" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="31" t="n">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="23" t="n">
         <v>45882</v>
       </c>
-      <c r="B17" s="32" t="n">
+      <c r="B17" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F17" s="32" t="s">
+      <c r="F17" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G17" s="32" t="s">
+      <c r="G17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="34" t="n">
+      <c r="H17" s="25" t="n">
         <v>31180</v>
       </c>
-      <c r="I17" s="34" t="n">
+      <c r="I17" s="25" t="n">
         <v>31180</v>
       </c>
-      <c r="J17" s="34" t="n">
+      <c r="J17" s="25" t="n">
         <v>43340</v>
       </c>
-      <c r="K17" s="35" t="n">
+      <c r="K17" s="26" t="n">
         <v>20</v>
       </c>
-      <c r="L17" s="32" t="s">
+      <c r="L17" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M17" s="36" t="s">
+      <c r="M17" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="N17" s="37" t="s">
+      <c r="N17" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="O17" s="33" t="s">
+      <c r="O17" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="P17" s="33" t="s">
+      <c r="P17" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="Q17" s="33" t="s">
+      <c r="Q17" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="R17" s="0"/>
     </row>
-    <row r="18" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="31" t="n">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="23" t="n">
         <v>30015</v>
       </c>
-      <c r="B18" s="32" t="n">
+      <c r="B18" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="34" t="n">
+      <c r="H18" s="25" t="n">
         <v>23410</v>
       </c>
-      <c r="I18" s="34" t="n">
+      <c r="I18" s="25" t="n">
         <v>23410</v>
       </c>
-      <c r="J18" s="34" t="n">
+      <c r="J18" s="25" t="n">
         <v>43552</v>
       </c>
-      <c r="K18" s="35" t="n">
+      <c r="K18" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="L18" s="32" t="s">
+      <c r="L18" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="M18" s="36" t="s">
+      <c r="M18" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="N18" s="37" t="s">
+      <c r="N18" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="O18" s="33" t="s">
+      <c r="O18" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="P18" s="33" t="s">
+      <c r="P18" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="Q18" s="33" t="s">
+      <c r="Q18" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="R18" s="0"/>
     </row>
-    <row r="19" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="31" t="n">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="23" t="n">
         <v>44625</v>
       </c>
-      <c r="B19" s="32" t="n">
+      <c r="B19" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="D19" s="32" t="s">
+      <c r="D19" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F19" s="32" t="s">
+      <c r="F19" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="G19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H19" s="34" t="n">
+      <c r="H19" s="25" t="n">
         <v>30098</v>
       </c>
-      <c r="I19" s="34" t="n">
+      <c r="I19" s="25" t="n">
         <v>30098</v>
       </c>
-      <c r="J19" s="34" t="n">
+      <c r="J19" s="25" t="n">
         <v>42842</v>
       </c>
-      <c r="K19" s="35" t="n">
+      <c r="K19" s="26" t="n">
         <v>59</v>
       </c>
-      <c r="L19" s="32" t="s">
+      <c r="L19" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="M19" s="36" t="s">
+      <c r="M19" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="N19" s="37" t="s">
+      <c r="N19" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="O19" s="33" t="s">
+      <c r="O19" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="P19" s="38" t="s">
+      <c r="P19" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="Q19" s="33" t="s">
+      <c r="Q19" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="R19" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:R7"/>
+  <autoFilter ref="A4:R11634"/>
   <mergeCells count="2">
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:D3"/>

</xml_diff>

<commit_message>
Use parslet for --calc. Still many failing unit tests
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -12,26 +12,28 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Sheet1!$3:$4</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="160">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -475,6 +477,51 @@
   </si>
   <si>
     <t>Infektionskrankheiten</t>
+  </si>
+  <si>
+    <t>Cefuroxim Actavis 250 mg, Filmtabletten</t>
+  </si>
+  <si>
+    <t>Actavis Switzerland AG</t>
+  </si>
+  <si>
+    <t>J01DC02</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>cefuroximum</t>
+  </si>
+  <si>
+    <t>cefuroximum 250 mg ut cefuroximum axetil, excipiens pro compresso obducto.</t>
+  </si>
+  <si>
+    <t>Glatiramer-Mepha, Fertigspritzen</t>
+  </si>
+  <si>
+    <t>Mepha Pharma AG</t>
+  </si>
+  <si>
+    <t>01.99.0.</t>
+  </si>
+  <si>
+    <t>L03AX13</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>Spritze(n)</t>
+  </si>
+  <si>
+    <t>glatiramerum</t>
+  </si>
+  <si>
+    <t>glatiramerum acetas 20 mg corresp. glatiramerum 18 mg, mannitolum, aqua ad iniectabilia q.s. ad solutionem pro 0.5 ml.</t>
+  </si>
+  <si>
+    <t>Multiple Sklerose</t>
   </si>
 </sst>
 </file>
@@ -583,7 +630,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -706,6 +753,34 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -725,15 +800,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>162000</xdr:colOff>
+      <xdr:colOff>189000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1074600</xdr:colOff>
+      <xdr:colOff>1101240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>541080</xdr:rowOff>
+      <xdr:rowOff>540720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -746,8 +821,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="162000" y="0"/>
-          <a:ext cx="1779120" cy="541080"/>
+          <a:off x="189000" y="0"/>
+          <a:ext cx="1778760" cy="540720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -767,12 +842,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1830" topLeftCell="A4" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="1605" topLeftCell="A4" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A21" activeCellId="0" sqref="21:21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1685,8 +1760,115 @@
         <v>144</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="31" t="n">
+        <v>65657</v>
+      </c>
+      <c r="B20" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="F20" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="G20" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="34" t="n">
+        <v>42025</v>
+      </c>
+      <c r="I20" s="34" t="n">
+        <v>42025</v>
+      </c>
+      <c r="J20" s="34" t="n">
+        <v>43850</v>
+      </c>
+      <c r="K20" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="M20" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="N20" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="O20" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="P20" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q20" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="R20" s="33"/>
+    </row>
+    <row r="21" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="31" t="n">
+        <v>65677</v>
+      </c>
+      <c r="B21" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="F21" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="G21" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="34" t="n">
+        <v>42051</v>
+      </c>
+      <c r="I21" s="34" t="n">
+        <v>42051</v>
+      </c>
+      <c r="J21" s="34" t="n">
+        <v>43876</v>
+      </c>
+      <c r="K21" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="M21" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="N21" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="O21" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="P21" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q21" s="33" t="s">
+        <v>159</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A4:R11634"/>
+  <autoFilter ref="A4:R7"/>
   <mergeCells count="2">
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:D3"/>

</xml_diff>

<commit_message>
Handle ratio: in oddb2xml --calc
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -12,7 +12,6 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Sheet1!$3:$4</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="159">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -86,7 +85,7 @@
     <t>Wirkstoff</t>
   </si>
   <si>
-    <t>Zusammensetzung</t>
+    <t>u</t>
   </si>
   <si>
     <t>Anwendungsgebiet Präparate</t>
@@ -129,145 +128,58 @@
 Possibilités d'emploi voir information professionnelle</t>
   </si>
   <si>
-    <t>nam</t>
-  </si>
-  <si>
-    <t>AstraZeneca AG</t>
-  </si>
-  <si>
-    <t>01.02.2.</t>
-  </si>
-  <si>
-    <t>N01BB09</t>
-  </si>
-  <si>
-    <t>Synthetika human</t>
-  </si>
-  <si>
-    <t>_:</t>
-  </si>
-  <si>
-    <t>,.</t>
-  </si>
-  <si>
-    <t>ropivacainum</t>
-  </si>
-  <si>
-    <t>ropivacaini hydrochloridum 2 mg, natrii chloridum, aqua ad iniectabilia q.s. ad solutionem pro 1 ml.</t>
-  </si>
-  <si>
-    <t>Lokalanästhetikum</t>
-  </si>
-  <si>
-    <t>Naropin 0,2 %, Infusionslösung / Injektionslösung</t>
-  </si>
-  <si>
-    <t>1 x 5 x 200</t>
-  </si>
-  <si>
-    <t>ml</t>
-  </si>
-  <si>
-    <t>W-Tropfen</t>
-  </si>
-  <si>
-    <t>Iromedica AG</t>
-  </si>
-  <si>
-    <t>10.07.0.</t>
-  </si>
-  <si>
-    <t>D11AF</t>
+    <t>Mutagrip, Suspension zur Injektion</t>
+  </si>
+  <si>
+    <t>Sanofi Pasteur MSD AG</t>
+  </si>
+  <si>
+    <t>08.08.</t>
+  </si>
+  <si>
+    <t>J07BB02</t>
+  </si>
+  <si>
+    <t>Impfstoffe</t>
+  </si>
+  <si>
+    <t>10 x 0.5 ml</t>
+  </si>
+  <si>
+    <t>Fertigspritze(n)</t>
+  </si>
+  <si>
+    <t>haemagglutininum influenzae A (H1N1) (Virus-Stamm A/California/7/2009 (H1N1)-like: reassortant virus NYMC X-179A), haemagglutininum influenzae A (H3N2) (Virus-Stamm A/Texas/50/2012 (H3N2)-like: reassortant virus NYMC X-223A), haemagglutininum influenzae B (Virus-Stamm B/Massachusetts/2/2012-like: B/Massachusetts/2/2012)</t>
+  </si>
+  <si>
+    <t>haemagglutininum influenzae A (H1N1) (Virus-Stamm A/California/7/2009 (H1N1)-like: reassortant virus NYMC X-179A) 15 µg, haemagglutininum influenzae A (H3N2) (Virus-Stamm A/Texas/50/2012 (H3N2)-like: reassortant virus NYMC X-223A) 15 µg, haemagglutininum influenzae B (Virus-Stamm B/Massachusetts/2/2012-like: B/Massachusetts/2/2012) 15 µg, natrii chloridum, kalii chloridum, dinatrii phosphas dihydricus, kalii dihydrogenophosphas, residui: formaldehydum max. 100 µg, octoxinolum-9 max. 500 µg, ovalbuminum max. 0.05 µg, saccharum nihil, neomycinum nihil, aqua ad iniectabilia q.s. ad suspensionem pro 0.5 ml.</t>
+  </si>
+  <si>
+    <t>aktive Immunisierung gegen Influenza, ab dem vollendeten 6. Lebensmonat</t>
+  </si>
+  <si>
+    <t>Infloran, capsule</t>
+  </si>
+  <si>
+    <t>Desma Healthcare SpA, Torino succursale di Chiasso</t>
+  </si>
+  <si>
+    <t>04.09.0.</t>
+  </si>
+  <si>
+    <t>A07FA01</t>
+  </si>
+  <si>
+    <t>Bakterien- und Hefepräparate</t>
+  </si>
+  <si>
+    <t>2x10</t>
+  </si>
+  <si>
+    <t>Kapsel(n)</t>
   </si>
   <si>
     <t>D</t>
-  </si>
-  <si>
-    <t>acidum lacticum, acidum salicylicum</t>
-  </si>
-  <si>
-    <t>acidum lacticum 40.915 mg, acidum salicylicum 100.2 mg, excipiens ad solutionem pro 1 ml.</t>
-  </si>
-  <si>
-    <t>Hühneraugen, Hornhaut, Warzen</t>
-  </si>
-  <si>
-    <t>Diamox, comprimés</t>
-  </si>
-  <si>
-    <t>Vifor SA</t>
-  </si>
-  <si>
-    <t>11.09.0.</t>
-  </si>
-  <si>
-    <t>S01EC01</t>
-  </si>
-  <si>
-    <t>1 x 25</t>
-  </si>
-  <si>
-    <t>Tablette(n)</t>
-  </si>
-  <si>
-    <t>acetazolamidum</t>
-  </si>
-  <si>
-    <t>acetazolamidum 250 mg, excipiens pro compresso.</t>
-  </si>
-  <si>
-    <t>inhibiteur de l'anhydrase carbonique</t>
-  </si>
-  <si>
-    <t>Mutagrip, Suspension zur Injektion</t>
-  </si>
-  <si>
-    <t>Sanofi Pasteur MSD AG</t>
-  </si>
-  <si>
-    <t>08.08.</t>
-  </si>
-  <si>
-    <t>J07BB02</t>
-  </si>
-  <si>
-    <t>Impfstoffe</t>
-  </si>
-  <si>
-    <t>10 x 0.5 ml</t>
-  </si>
-  <si>
-    <t>Fertigspritze(n)</t>
-  </si>
-  <si>
-    <t>haemagglutininum influenzae A (H1N1) (Virus-Stamm A/California/7/2009 (H1N1)-like: reassortant virus NYMC X-179A), haemagglutininum influenzae A (H3N2) (Virus-Stamm A/Texas/50/2012 (H3N2)-like: reassortant virus NYMC X-223A), haemagglutininum influenzae B (Virus-Stamm B/Massachusetts/2/2012-like: B/Massachusetts/2/2012)</t>
-  </si>
-  <si>
-    <t>haemagglutininum influenzae A (H1N1) (Virus-Stamm A/California/7/2009 (H1N1)-like: reassortant virus NYMC X-179A) 15 µg, haemagglutininum influenzae A (H3N2) (Virus-Stamm A/Texas/50/2012 (H3N2)-like: reassortant virus NYMC X-223A) 15 µg, haemagglutininum influenzae B (Virus-Stamm B/Massachusetts/2/2012-like: B/Massachusetts/2/2012) 15 µg, natrii chloridum, kalii chloridum, dinatrii phosphas dihydricus, kalii dihydrogenophosphas, residui: formaldehydum max. 100 µg, octoxinolum-9 max. 500 µg, ovalbuminum max. 0.05 µg, saccharum nihil, neomycinum nihil, aqua ad iniectabilia q.s. ad suspensionem pro 0.5 ml.</t>
-  </si>
-  <si>
-    <t>aktive Immunisierung gegen Influenza, ab dem vollendeten 6. Lebensmonat</t>
-  </si>
-  <si>
-    <t>Infloran, capsule</t>
-  </si>
-  <si>
-    <t>Desma Healthcare SpA, Torino succursale di Chiasso</t>
-  </si>
-  <si>
-    <t>04.09.0.</t>
-  </si>
-  <si>
-    <t>A07FA01</t>
-  </si>
-  <si>
-    <t>Bakterien- und Hefepräparate</t>
-  </si>
-  <si>
-    <t>2x10</t>
-  </si>
-  <si>
-    <t>Kapsel(n)</t>
   </si>
   <si>
     <t>lactobacillus acidophilus cryodesiccatus, bifidobacterium infantis</t>
@@ -280,6 +192,108 @@
 Trattamento sintomatico della diarrea</t>
   </si>
   <si>
+    <t>Lapidar 4, Filmtabletten</t>
+  </si>
+  <si>
+    <t>Kräuterpfarrer Künzle AG</t>
+  </si>
+  <si>
+    <t>02.08.1.</t>
+  </si>
+  <si>
+    <t>C05CA51</t>
+  </si>
+  <si>
+    <t>Synthetika human</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>Tablette(n)</t>
+  </si>
+  <si>
+    <t>rutosidum trihydricum, aescinum</t>
+  </si>
+  <si>
+    <t>rutosidum trihydricum 20 mg, aescinum 25 mg, aromatica, excipiens pro compresso.</t>
+  </si>
+  <si>
+    <t>Symptome bei Krampfadern</t>
+  </si>
+  <si>
+    <t>W-Tropfen</t>
+  </si>
+  <si>
+    <t>Iromedica AG</t>
+  </si>
+  <si>
+    <t>10.07.0.</t>
+  </si>
+  <si>
+    <t>D11AF</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t>acidum lacticum, acidum salicylicum</t>
+  </si>
+  <si>
+    <t>acidum lacticum 40.915 mg, acidum salicylicum 100.2 mg, excipiens ad solutionem pro 1 ml.</t>
+  </si>
+  <si>
+    <t>Hühneraugen, Hornhaut, Warzen</t>
+  </si>
+  <si>
+    <t>Diamox, comprimés</t>
+  </si>
+  <si>
+    <t>Vifor SA</t>
+  </si>
+  <si>
+    <t>11.09.0.</t>
+  </si>
+  <si>
+    <t>S01EC01</t>
+  </si>
+  <si>
+    <t>1 x 25</t>
+  </si>
+  <si>
+    <t>acetazolamidum</t>
+  </si>
+  <si>
+    <t>acetazolamidum 250 mg, excipiens pro compresso.</t>
+  </si>
+  <si>
+    <t>inhibiteur de l'anhydrase carbonique</t>
+  </si>
+  <si>
+    <t>Lidocain 1% Streuli, Injektionslösung (Ampullen)</t>
+  </si>
+  <si>
+    <t>Streuli Pharma AG</t>
+  </si>
+  <si>
+    <t>01.02.2.</t>
+  </si>
+  <si>
+    <t>N01BB02</t>
+  </si>
+  <si>
+    <t>10 x  2</t>
+  </si>
+  <si>
+    <t>lidocaini hydrochloridum</t>
+  </si>
+  <si>
+    <t>lidocaini hydrochloridum 10 mg, natrii chloridum, aqua ad iniectabilia q.s. ad solutionem pro 1 ml.</t>
+  </si>
+  <si>
+    <t>Lokalanaestheticum</t>
+  </si>
+  <si>
     <t>Kamillin Medipharm, Bad</t>
   </si>
   <si>
@@ -304,29 +318,89 @@
     <t>Bei Hauterkrankungen</t>
   </si>
   <si>
-    <t>bicaNova 1,5 % Glucose, Peritonealdialyselösung</t>
-  </si>
-  <si>
-    <t>Fresenius Medical Care (Schweiz) AG</t>
-  </si>
-  <si>
-    <t>05.04.0.</t>
-  </si>
-  <si>
-    <t>B05DB</t>
-  </si>
-  <si>
-    <t>1500 ml</t>
-  </si>
-  <si>
-    <t>natrii chloridum, natrii hydrogenocarbonas, calcii chloridum dihydricum, magnesii chloridum hexahydricum, glucosum anhydricum, natrium, calcium, magnesium, chloridum, hydrogenocarbonas, glucosum</t>
-  </si>
-  <si>
-    <t>I) et II) corresp.: natrii chloridum 5.5 g, natrii hydrogenocarbonas 3.36 g, calcii chloridum dihydricum 184 mg, magnesii chloridum hexahydricum 102 mg, glucosum anhydricum 15 g ut glucosum monohydricum, aqua ad iniectabilia q.s. ad solutionem pro 1000 ml.
-Corresp. natrium 134 mmol, calcium 1.25 mmol, magnesium 0.5 mmol, chloridum 98.5 mmol, hydrogenocarbonas 39 mmol, glucosum 83.25 mmol.</t>
-  </si>
-  <si>
-    <t>Peritonealdialyse</t>
+    <t>Rocephin 500 mg i.v., Trockenampullen + Solvens</t>
+  </si>
+  <si>
+    <t>Roche Pharma (Schweiz) AG</t>
+  </si>
+  <si>
+    <t>08.01.3.</t>
+  </si>
+  <si>
+    <t>J01DD04</t>
+  </si>
+  <si>
+    <t>5 + 5</t>
+  </si>
+  <si>
+    <t>Ampulle(n)</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>ceftriaxonum</t>
+  </si>
+  <si>
+    <t>Praeparatio sicca: ceftriaxonum 500 mg ut ceftriaxonum natricum pro vitro.
+Solvens: aqua ad iniectabilia 5 ml.</t>
+  </si>
+  <si>
+    <t>Infektionskrankheiten</t>
+  </si>
+  <si>
+    <t>Magnesiumchlorid 0,5 molar B. Braun, Zusatzampulle für              Infusionslösungen</t>
+  </si>
+  <si>
+    <t>B. Braun Medical AG</t>
+  </si>
+  <si>
+    <t>05.03.2.</t>
+  </si>
+  <si>
+    <t>B05XA11</t>
+  </si>
+  <si>
+    <t>5 x 10 mL</t>
+  </si>
+  <si>
+    <t>magnesium, chloridum</t>
+  </si>
+  <si>
+    <t>magnesium 500 mmol, chloridum 1000 mmol, aqua ad iniectabilia q.s. ad solutionem pro 1000 ml.</t>
+  </si>
+  <si>
+    <t>Magnesiummangel</t>
+  </si>
+  <si>
+    <t>nam</t>
+  </si>
+  <si>
+    <t>AstraZeneca AG</t>
+  </si>
+  <si>
+    <t>N01BB09</t>
+  </si>
+  <si>
+    <t>_:</t>
+  </si>
+  <si>
+    <t>,.</t>
+  </si>
+  <si>
+    <t>ropivacainum</t>
+  </si>
+  <si>
+    <t>ropivacaini hydrochloridum 2 mg, natrii chloridum, aqua ad iniectabilia q.s. ad solutionem pro 1 ml.</t>
+  </si>
+  <si>
+    <t>Lokalanästhetikum</t>
+  </si>
+  <si>
+    <t>Naropin 0,2 %, Infusionslösung / Injektionslösung</t>
+  </si>
+  <si>
+    <t>1 x 5 x 200</t>
   </si>
   <si>
     <t>Muse 125 ug, Urethrastab</t>
@@ -354,9 +428,6 @@
   </si>
   <si>
     <t>Nutriflex Lipid plus, Infusionsemulsion, 1250ml</t>
-  </si>
-  <si>
-    <t>B. Braun Medical AG</t>
   </si>
   <si>
     <t>07.01.2.</t>
@@ -382,101 +453,53 @@
     <t>Parenterale Ernährung</t>
   </si>
   <si>
-    <t>Lapidar 4, Filmtabletten</t>
-  </si>
-  <si>
-    <t>Kräuterpfarrer Künzle AG</t>
-  </si>
-  <si>
-    <t>02.08.1.</t>
-  </si>
-  <si>
-    <t>C05CA51</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>rutosidum trihydricum, aescinum</t>
-  </si>
-  <si>
-    <t>rutosidum trihydricum 20 mg, aescinum 25 mg, aromatica, excipiens pro compresso.</t>
-  </si>
-  <si>
-    <t>Symptome bei Krampfadern</t>
-  </si>
-  <si>
-    <t>Magnesiumchlorid 0,5 molar B. Braun, Zusatzampulle für              Infusionslösungen</t>
-  </si>
-  <si>
-    <t>05.03.2.</t>
-  </si>
-  <si>
-    <t>B05XA11</t>
-  </si>
-  <si>
-    <t>5 x 10 mL</t>
-  </si>
-  <si>
-    <t>Ampulle(n)</t>
-  </si>
-  <si>
-    <t>magnesium, chloridum</t>
-  </si>
-  <si>
-    <t>magnesium 500 mmol, chloridum 1000 mmol, aqua ad iniectabilia q.s. ad solutionem pro 1000 ml.</t>
-  </si>
-  <si>
-    <t>Magnesiummangel</t>
-  </si>
-  <si>
-    <t>Lidocain 1% Streuli, Injektionslösung (Ampullen)</t>
-  </si>
-  <si>
-    <t>Streuli Pharma AG</t>
-  </si>
-  <si>
-    <t>N01BB02</t>
-  </si>
-  <si>
-    <t>10 x  2</t>
-  </si>
-  <si>
-    <t>lidocaini hydrochloridum</t>
-  </si>
-  <si>
-    <t>lidocaini hydrochloridum 10 mg, natrii chloridum, aqua ad iniectabilia q.s. ad solutionem pro 1 ml.</t>
-  </si>
-  <si>
-    <t>Lokalanaestheticum</t>
-  </si>
-  <si>
-    <t>Rocephin 500 mg i.v., Trockenampullen + Solvens</t>
-  </si>
-  <si>
-    <t>Roche Pharma (Schweiz) AG</t>
-  </si>
-  <si>
-    <t>08.01.3.</t>
-  </si>
-  <si>
-    <t>J01DD04</t>
-  </si>
-  <si>
-    <t>5 + 5</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>ceftriaxonum</t>
-  </si>
-  <si>
-    <t>Praeparatio sicca: ceftriaxonum 500 mg ut ceftriaxonum natricum pro vitro.
-Solvens: aqua ad iniectabilia 5 ml.</t>
-  </si>
-  <si>
-    <t>Infektionskrankheiten</t>
+    <t>bicaNova 1,5 % Glucose, Peritonealdialyselösung</t>
+  </si>
+  <si>
+    <t>Fresenius Medical Care (Schweiz) AG</t>
+  </si>
+  <si>
+    <t>05.04.0.</t>
+  </si>
+  <si>
+    <t>B05DB</t>
+  </si>
+  <si>
+    <t>1500 ml</t>
+  </si>
+  <si>
+    <t>natrii chloridum, natrii hydrogenocarbonas, calcii chloridum dihydricum, magnesii chloridum hexahydricum, glucosum anhydricum, natrium, calcium, magnesium, chloridum, hydrogenocarbonas, glucosum</t>
+  </si>
+  <si>
+    <t>I) et II) corresp.: natrii chloridum 5.5 g, natrii hydrogenocarbonas 3.36 g, calcii chloridum dihydricum 184 mg, magnesii chloridum hexahydricum 102 mg, glucosum anhydricum 15 g ut glucosum monohydricum, aqua ad iniectabilia q.s. ad solutionem pro 1000 ml.
+Corresp. natrium 134 mmol, calcium 1.25 mmol, magnesium 0.5 mmol, chloridum 98.5 mmol, hydrogenocarbonas 39 mmol, glucosum 83.25 mmol.</t>
+  </si>
+  <si>
+    <t>Peritonealdialyse</t>
+  </si>
+  <si>
+    <t>Viperfav 2500U , Infusionslösung</t>
+  </si>
+  <si>
+    <t>15.01.0.</t>
+  </si>
+  <si>
+    <t>J06AA03</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Durchstechflasche(n)</t>
+  </si>
+  <si>
+    <t>Solutio concentrata: viperis antitoxinum equis F(ab')2 corresp. Vipera aspis &gt; 1000 LD50 mus et Vipera berus &gt; 500 LD50 mus et Vipera ammodytes &gt; 1000 LD50 mus, natrii chloridum, polysorbatum 80, aqua ad iniectabilia q.s. ad solutionem pro 4 ml.</t>
+  </si>
+  <si>
+    <t>Antidot bei Viper Schlangenbiss</t>
+  </si>
+  <si>
+    <t>Schlangen-Biss durch europäische Viper (Vipera aspis, Vipera berus, Vipera ammodytes)</t>
   </si>
   <si>
     <t>Cefuroxim Actavis 250 mg, Filmtabletten</t>
@@ -495,33 +518,6 @@
   </si>
   <si>
     <t>cefuroximum 250 mg ut cefuroximum axetil, excipiens pro compresso obducto.</t>
-  </si>
-  <si>
-    <t>Glatiramer-Mepha, Fertigspritzen</t>
-  </si>
-  <si>
-    <t>Mepha Pharma AG</t>
-  </si>
-  <si>
-    <t>01.99.0.</t>
-  </si>
-  <si>
-    <t>L03AX13</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>Spritze(n)</t>
-  </si>
-  <si>
-    <t>glatiramerum</t>
-  </si>
-  <si>
-    <t>glatiramerum acetas 20 mg corresp. glatiramerum 18 mg, mannitolum, aqua ad iniectabilia q.s. ad solutionem pro 0.5 ml.</t>
-  </si>
-  <si>
-    <t>Multiple Sklerose</t>
   </si>
 </sst>
 </file>
@@ -845,9 +841,9 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1605" topLeftCell="A4" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="1605" topLeftCell="A1" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A21" activeCellId="0" sqref="21:21"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="5:21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1018,14 +1014,14 @@
       </c>
       <c r="R5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="n">
-        <v>54015</v>
+        <v>373</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1041,302 +1037,302 @@
         <v>35</v>
       </c>
       <c r="H6" s="25" t="n">
-        <v>35488</v>
+        <v>27661</v>
       </c>
       <c r="I6" s="25" t="n">
-        <v>35488</v>
+        <v>41835</v>
       </c>
       <c r="J6" s="25" t="n">
-        <v>42921</v>
+        <v>42916</v>
       </c>
       <c r="K6" s="26" t="n">
-        <v>100</v>
-      </c>
-      <c r="L6" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="0" t="s">
+      <c r="O6" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="P6" s="0" t="s">
+      <c r="P6" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="Q6" s="24" t="s">
         <v>40</v>
       </c>
+      <c r="R6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="n">
-        <v>54015</v>
+        <v>679</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>41</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="H7" s="25" t="n">
-        <v>35488</v>
+        <v>28230</v>
       </c>
       <c r="I7" s="25" t="n">
-        <v>35488</v>
+        <v>41599</v>
       </c>
       <c r="J7" s="25" t="n">
-        <v>42921</v>
+        <v>43247</v>
       </c>
       <c r="K7" s="26" t="n">
-        <v>119</v>
+        <v>12</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="P7" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q7" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+      <c r="M7" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="P7" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q7" s="29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="n">
-        <v>16598</v>
+        <v>10386</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="25" t="n">
+        <v>13027</v>
+      </c>
+      <c r="I8" s="25" t="n">
+        <v>13027</v>
+      </c>
+      <c r="J8" s="25" t="n">
+        <v>42358</v>
+      </c>
+      <c r="K8" s="26" t="n">
         <v>47</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="25" t="n">
-        <v>18833</v>
-      </c>
-      <c r="I8" s="25" t="n">
-        <v>18833</v>
-      </c>
-      <c r="J8" s="25" t="n">
-        <v>43085</v>
-      </c>
-      <c r="K8" s="26" t="n">
-        <v>11</v>
-      </c>
-      <c r="L8" s="1" t="n">
-        <v>43454</v>
+      <c r="L8" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="M8" s="27" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="N8" s="28" t="s">
         <v>48</v>
       </c>
       <c r="O8" s="24" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="Q8" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="R8" s="0"/>
+        <v>61</v>
+      </c>
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="n">
-        <v>21191</v>
+        <v>16598</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="H9" s="25" t="n">
-        <v>20325</v>
+        <v>18833</v>
       </c>
       <c r="I9" s="25" t="n">
-        <v>20325</v>
+        <v>18833</v>
       </c>
       <c r="J9" s="25" t="n">
-        <v>43667</v>
+        <v>43085</v>
       </c>
       <c r="K9" s="26" t="n">
-        <v>19</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>56</v>
+        <v>11</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>43454</v>
       </c>
       <c r="M9" s="27" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="N9" s="28" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="O9" s="24" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="P9" s="24" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="Q9" s="24" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="R9" s="0"/>
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="n">
-        <v>373</v>
+        <v>21191</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="H10" s="25" t="n">
-        <v>27661</v>
+        <v>20325</v>
       </c>
       <c r="I10" s="25" t="n">
-        <v>41835</v>
+        <v>20325</v>
       </c>
       <c r="J10" s="25" t="n">
-        <v>42916</v>
+        <v>43667</v>
       </c>
       <c r="K10" s="26" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="M10" s="27" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="N10" s="28" t="s">
         <v>27</v>
       </c>
       <c r="O10" s="24" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="P10" s="24" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="Q10" s="24" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="R10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="n">
-        <v>679</v>
+        <v>30015</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="H11" s="25" t="n">
-        <v>28230</v>
+        <v>23410</v>
       </c>
       <c r="I11" s="25" t="n">
-        <v>41599</v>
+        <v>23410</v>
       </c>
       <c r="J11" s="25" t="n">
-        <v>43247</v>
+        <v>43552</v>
       </c>
       <c r="K11" s="26" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="M11" s="27" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="N11" s="28" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="O11" s="24" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="P11" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q11" s="29" t="s">
-        <v>80</v>
+        <v>84</v>
+      </c>
+      <c r="Q11" s="24" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1347,19 +1343,19 @@
         <v>1</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H12" s="25" t="n">
         <v>29650</v>
@@ -1374,381 +1370,381 @@
         <v>101</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M12" s="27" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="N12" s="28" t="s">
         <v>48</v>
       </c>
       <c r="O12" s="24" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="P12" s="24" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="Q12" s="24" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="n">
-        <v>58277</v>
+        <v>44625</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="H13" s="25" t="n">
-        <v>39638</v>
+        <v>30098</v>
       </c>
       <c r="I13" s="25" t="n">
-        <v>39638</v>
+        <v>30098</v>
       </c>
       <c r="J13" s="25" t="n">
-        <v>43289</v>
+        <v>42842</v>
       </c>
       <c r="K13" s="26" t="n">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M13" s="0"/>
+        <v>98</v>
+      </c>
+      <c r="M13" s="27" t="s">
+        <v>99</v>
+      </c>
       <c r="N13" s="28" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="O13" s="24" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="P13" s="29" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="Q13" s="24" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="n">
-        <v>54525</v>
+        <v>45882</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="25" t="n">
+        <v>31180</v>
+      </c>
+      <c r="I14" s="25" t="n">
+        <v>31180</v>
+      </c>
+      <c r="J14" s="25" t="n">
+        <v>43340</v>
+      </c>
+      <c r="K14" s="26" t="n">
+        <v>20</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M14" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" s="25" t="n">
-        <v>35852</v>
-      </c>
-      <c r="I14" s="25" t="n">
-        <v>35852</v>
-      </c>
-      <c r="J14" s="25" t="n">
-        <v>43553</v>
-      </c>
-      <c r="K14" s="26" t="n">
-        <v>36</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="M14" s="0"/>
       <c r="N14" s="28" t="s">
         <v>27</v>
       </c>
       <c r="O14" s="24" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="P14" s="24" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="Q14" s="24" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="n">
-        <v>55594</v>
+        <v>54015</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="24" t="s">
-        <v>105</v>
+      <c r="C15" s="0" t="s">
+        <v>112</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="H15" s="25" t="n">
-        <v>37172</v>
+        <v>35488</v>
       </c>
       <c r="I15" s="25" t="n">
-        <v>37172</v>
+        <v>35488</v>
       </c>
       <c r="J15" s="25" t="n">
-        <v>43863</v>
+        <v>42921</v>
       </c>
       <c r="K15" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="M15" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="N15" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="L15" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="N15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="O15" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="P15" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q15" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="R15" s="0"/>
+      <c r="O15" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="P15" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q15" s="0" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="n">
-        <v>10386</v>
+        <v>54015</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="H16" s="25" t="n">
-        <v>13027</v>
+        <v>35488</v>
       </c>
       <c r="I16" s="25" t="n">
-        <v>13027</v>
+        <v>35488</v>
       </c>
       <c r="J16" s="25" t="n">
-        <v>42358</v>
+        <v>42921</v>
       </c>
       <c r="K16" s="26" t="n">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="L16" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O16" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="M16" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="N16" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="O16" s="24" t="s">
+      <c r="P16" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="P16" s="24" t="s">
+      <c r="Q16" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="Q16" s="24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="23" t="n">
-        <v>45882</v>
+        <v>54525</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="H17" s="25" t="n">
-        <v>31180</v>
+        <v>35852</v>
       </c>
       <c r="I17" s="25" t="n">
-        <v>31180</v>
+        <v>35852</v>
       </c>
       <c r="J17" s="25" t="n">
-        <v>43340</v>
+        <v>43553</v>
       </c>
       <c r="K17" s="26" t="n">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M17" s="27" t="s">
-        <v>125</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="M17" s="0"/>
       <c r="N17" s="28" t="s">
         <v>27</v>
       </c>
       <c r="O17" s="24" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="P17" s="24" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Q17" s="24" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="n">
-        <v>30015</v>
+        <v>55594</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>33</v>
+        <v>131</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="H18" s="25" t="n">
-        <v>23410</v>
+        <v>37172</v>
       </c>
       <c r="I18" s="25" t="n">
-        <v>23410</v>
+        <v>37172</v>
       </c>
       <c r="J18" s="25" t="n">
-        <v>43552</v>
+        <v>43863</v>
       </c>
       <c r="K18" s="26" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="M18" s="27" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="N18" s="28" t="s">
         <v>27</v>
       </c>
       <c r="O18" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="P18" s="24" t="s">
         <v>134</v>
       </c>
+      <c r="P18" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="Q18" s="24" t="s">
-        <v>135</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="R18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="23" t="n">
-        <v>44625</v>
+        <v>58277</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="H19" s="25" t="n">
-        <v>30098</v>
+        <v>39638</v>
       </c>
       <c r="I19" s="25" t="n">
-        <v>30098</v>
+        <v>39638</v>
       </c>
       <c r="J19" s="25" t="n">
-        <v>42842</v>
+        <v>43289</v>
       </c>
       <c r="K19" s="26" t="n">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="M19" s="27" t="s">
-        <v>125</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="M19" s="0"/>
       <c r="N19" s="28" t="s">
-        <v>141</v>
+        <v>27</v>
       </c>
       <c r="O19" s="24" t="s">
         <v>142</v>
@@ -1760,9 +1756,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="31" t="n">
-        <v>65657</v>
+        <v>65628</v>
       </c>
       <c r="B20" s="32" t="n">
         <v>1</v>
@@ -1771,25 +1767,25 @@
         <v>145</v>
       </c>
       <c r="D20" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="32" t="s">
         <v>146</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>138</v>
       </c>
       <c r="F20" s="32" t="s">
         <v>147</v>
       </c>
       <c r="G20" s="32" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="H20" s="34" t="n">
-        <v>42025</v>
+        <v>41991</v>
       </c>
       <c r="I20" s="34" t="n">
-        <v>42025</v>
+        <v>41991</v>
       </c>
       <c r="J20" s="34" t="n">
-        <v>43850</v>
+        <v>43816</v>
       </c>
       <c r="K20" s="35" t="n">
         <v>1</v>
@@ -1798,64 +1794,64 @@
         <v>148</v>
       </c>
       <c r="M20" s="36" t="s">
-        <v>57</v>
+        <v>149</v>
       </c>
       <c r="N20" s="37" t="s">
-        <v>141</v>
-      </c>
-      <c r="O20" s="33" t="s">
-        <v>149</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="O20" s="0"/>
       <c r="P20" s="33" t="s">
         <v>150</v>
       </c>
       <c r="Q20" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="R20" s="33"/>
-    </row>
-    <row r="21" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>151</v>
+      </c>
+      <c r="R20" s="33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="31" t="n">
-        <v>65677</v>
+        <v>65657</v>
       </c>
       <c r="B21" s="32" t="n">
         <v>1</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>153</v>
+        <v>96</v>
       </c>
       <c r="F21" s="32" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="H21" s="34" t="n">
-        <v>42051</v>
+        <v>42025</v>
       </c>
       <c r="I21" s="34" t="n">
-        <v>42051</v>
+        <v>42025</v>
       </c>
       <c r="J21" s="34" t="n">
-        <v>43876</v>
+        <v>43850</v>
       </c>
       <c r="K21" s="35" t="n">
         <v>1</v>
       </c>
       <c r="L21" s="32" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="M21" s="36" t="s">
-        <v>156</v>
+        <v>58</v>
       </c>
       <c r="N21" s="37" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="O21" s="33" t="s">
         <v>157</v>
@@ -1864,11 +1860,11 @@
         <v>158</v>
       </c>
       <c r="Q21" s="33" t="s">
-        <v>159</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="R21" s="33"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:R7"/>
   <mergeCells count="2">
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:D3"/>

</xml_diff>

<commit_message>
Output more fields when running --calc
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="164">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -518,6 +518,26 @@
   </si>
   <si>
     <t>cefuroximum 250 mg ut cefuroximum axetil, excipiens pro compresso obducto.</t>
+  </si>
+  <si>
+    <t>Nutriflex Omega special, Infusionsemulsion 2500 ml</t>
+  </si>
+  <si>
+    <t>5 x 2500 ml</t>
+  </si>
+  <si>
+    <t>Beutel</t>
+  </si>
+  <si>
+    <t>glucosum anhydricum, natrii dihydrogenophosphas dihydricus, zinci acetas dihydricus, isoleucinum, leucinum, lysinum anhydricum, methioninum, phenylalaninum, threoninum, tryptophanum, valinum, argininum, histidinum, alaninum, acidum asparticum, acidum glutamicum, glycinum, prolinum, serinum, natrii hydroxidum, natrii chloridum, natrii acetas trihydricus, kalii acetas, magnesii acetas tetrahydricus, calcii chloridum dihydricum, aminoacida, nitrogenia, carbohydrata, materia crassa, natrium, kalium, magnesium, calcium, zincum, chloridum, phosphas, acetas, sojae oleum, triglycerida saturata media, omega-3 acidorum triglycerida</t>
+  </si>
+  <si>
+    <t>I) Glucoselösung: glucosum anhydricum 360 g ut glucosum monohydricum, natrii dihydrogenophosphas dihydricus 6.24 g, zinci acetas dihydricus 17.56 mg, aqua ad iniectabilia q.s. ad solutionem pro 1000 ml.
+II) Fettemulsion: sojae oleum 40 g, triglycerida saturata media 50 g, omega-3 acidorum triglycerida 10 g, glycerolum, lecithinum ex ovo, natrii oleas, antiox.: E 307 100 mg, aqua ad iniectabilia q.s. ad emulsionem pro 500 ml.
+III) Aminosäurenlösung: isoleucinum 8.21 g, leucinum 10.96 g, lysinum anhydricum 7.95 g ut lysinum monohydricum, methioninum 6.84 g, phenylalaninum 12.29 g, threoninum 6.35 g, tryptophanum 2 g, valinum 9.01 g, argininum 9.45 g, histidinum 4.38 g ut histidini hydrochloridum monohydricum, alaninum 16.98 g, acidum asparticum 5.25 g, acidum glutamicum 12.27 g, glycinum 5.78 g, prolinum 11.9 g, serinum 10.5 g, natrii hydroxidum 2.928 g, natrii chloridum 946 mg, natrii acetas trihydricus 626 mg, kalii acetas 9.222 g, magnesii acetas tetrahydricus 2.274 g, calcii chloridum dihydricum 1.558 g, aqua ad iniectabilia q.s. ad solutionem pro 1000 ml.
+.
+I) et II) et III) corresp.: aminoacida 57.44 g/l, nitrogenia 8 g/l, carbohydrata 144 g/l, materia crassa 40 g/l, natrium 53.6 mmol/l, kalium 37.6 mmol/l, magnesium 4.24 mmol/l, calcium 4.24 mmol/l, zincum 0.032 mmol/l, chloridum 48 mmol/l, phosphas 16 mmol/l, acetas 48 mmol/l, in emulsione recenter mixta 1000 ml.
+Corresp. 4941 kJ pro 1 l.</t>
   </si>
 </sst>
 </file>
@@ -626,7 +646,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -777,6 +797,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -838,12 +862,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1605" topLeftCell="A1" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="5:21"/>
+      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="22:22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1864,6 +1888,60 @@
       </c>
       <c r="R21" s="33"/>
     </row>
+    <row r="22" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="31" t="n">
+        <v>61186</v>
+      </c>
+      <c r="B22" s="32" t="n">
+        <v>4</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="H22" s="34" t="n">
+        <v>40522</v>
+      </c>
+      <c r="I22" s="34" t="n">
+        <v>40522</v>
+      </c>
+      <c r="J22" s="34" t="n">
+        <v>42347</v>
+      </c>
+      <c r="K22" s="35" t="n">
+        <v>4</v>
+      </c>
+      <c r="L22" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="M22" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="N22" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="O22" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="P22" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q22" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="R22" s="0"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:M2"/>

</xml_diff>

<commit_message>
Fixed some pending tests. Better handling of galenic_forms
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -19,6 +19,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="172">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -538,6 +539,31 @@
 .
 I) et II) et III) corresp.: aminoacida 57.44 g/l, nitrogenia 8 g/l, carbohydrata 144 g/l, materia crassa 40 g/l, natrium 53.6 mmol/l, kalium 37.6 mmol/l, magnesium 4.24 mmol/l, calcium 4.24 mmol/l, zincum 0.032 mmol/l, chloridum 48 mmol/l, phosphas 16 mmol/l, acetas 48 mmol/l, in emulsione recenter mixta 1000 ml.
 Corresp. 4941 kJ pro 1 l.</t>
+  </si>
+  <si>
+    <t>Apligraf</t>
+  </si>
+  <si>
+    <t>Organogenesis Switzerland GmbH</t>
+  </si>
+  <si>
+    <t>10.06.0.</t>
+  </si>
+  <si>
+    <t>Transplantat: Gewebeprodukt</t>
+  </si>
+  <si>
+    <t>75 mm</t>
+  </si>
+  <si>
+    <t>Scheibe(n)/disque(s)</t>
+  </si>
+  <si>
+    <t>Wundbehandlung (Hautäquivalent)</t>
+  </si>
+  <si>
+    <t>Behandlung von chronischen venösen Beinulzera sowie von diabetischen Fussulzera 
+Behandlung von Muco-Gingivalen Läsionen (Anwendung nur nach  Herstellung  mit Rinderhypophysenextrakt aus einem Land Kategorie A)</t>
   </si>
 </sst>
 </file>
@@ -820,15 +846,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>189000</xdr:colOff>
+      <xdr:colOff>216000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1101240</xdr:colOff>
+      <xdr:colOff>1127880</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>540720</xdr:rowOff>
+      <xdr:rowOff>540360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -841,8 +867,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="189000" y="0"/>
-          <a:ext cx="1778760" cy="540720"/>
+          <a:off x="216000" y="0"/>
+          <a:ext cx="1778400" cy="540360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -862,12 +888,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1605" topLeftCell="A1" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="22:22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1410" topLeftCell="A1" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="M23" activeCellId="0" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1038,7 +1064,7 @@
       </c>
       <c r="R5" s="0"/>
     </row>
-    <row r="6" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="n">
         <v>373</v>
       </c>
@@ -1090,7 +1116,6 @@
       <c r="Q6" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="R6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="n">
@@ -1780,167 +1805,217 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="31" t="n">
+    <row r="20" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="23" t="n">
         <v>65628</v>
       </c>
-      <c r="B20" s="32" t="n">
+      <c r="B20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="32" t="s">
+      <c r="E20" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F20" s="32" t="s">
+      <c r="F20" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G20" s="32" t="s">
+      <c r="G20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="34" t="n">
+      <c r="H20" s="25" t="n">
         <v>41991</v>
       </c>
-      <c r="I20" s="34" t="n">
+      <c r="I20" s="25" t="n">
         <v>41991</v>
       </c>
-      <c r="J20" s="34" t="n">
+      <c r="J20" s="25" t="n">
         <v>43816</v>
       </c>
-      <c r="K20" s="35" t="n">
+      <c r="K20" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="L20" s="32" t="s">
+      <c r="L20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="M20" s="36" t="s">
+      <c r="M20" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="N20" s="37" t="s">
+      <c r="N20" s="28" t="s">
         <v>100</v>
       </c>
       <c r="O20" s="0"/>
-      <c r="P20" s="33" t="s">
+      <c r="P20" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="Q20" s="33" t="s">
+      <c r="Q20" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="R20" s="33" t="s">
+      <c r="R20" s="24" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="31" t="n">
+      <c r="A21" s="23" t="n">
         <v>65657</v>
       </c>
-      <c r="B21" s="32" t="n">
+      <c r="B21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G21" s="32" t="s">
+      <c r="G21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H21" s="34" t="n">
+      <c r="H21" s="25" t="n">
         <v>42025</v>
       </c>
-      <c r="I21" s="34" t="n">
+      <c r="I21" s="25" t="n">
         <v>42025</v>
       </c>
-      <c r="J21" s="34" t="n">
+      <c r="J21" s="25" t="n">
         <v>43850</v>
       </c>
-      <c r="K21" s="35" t="n">
+      <c r="K21" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="L21" s="32" t="s">
+      <c r="L21" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="M21" s="36" t="s">
+      <c r="M21" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="N21" s="37" t="s">
+      <c r="N21" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="O21" s="33" t="s">
+      <c r="O21" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="P21" s="33" t="s">
+      <c r="P21" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="Q21" s="33" t="s">
+      <c r="Q21" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="R21" s="33"/>
-    </row>
-    <row r="22" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="31" t="n">
+      <c r="R21" s="24"/>
+    </row>
+    <row r="22" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="23" t="n">
         <v>61186</v>
       </c>
-      <c r="B22" s="32" t="n">
+      <c r="B22" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E22" s="32" t="s">
+      <c r="E22" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F22" s="32" t="s">
+      <c r="F22" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="G22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H22" s="34" t="n">
+      <c r="H22" s="25" t="n">
         <v>40522</v>
       </c>
-      <c r="I22" s="34" t="n">
+      <c r="I22" s="25" t="n">
         <v>40522</v>
       </c>
-      <c r="J22" s="34" t="n">
+      <c r="J22" s="25" t="n">
         <v>42347</v>
       </c>
-      <c r="K22" s="35" t="n">
+      <c r="K22" s="26" t="n">
         <v>4</v>
       </c>
-      <c r="L22" s="32" t="s">
+      <c r="L22" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="M22" s="36" t="s">
+      <c r="M22" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="N22" s="37" t="s">
+      <c r="N22" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="O22" s="33" t="s">
+      <c r="O22" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="P22" s="38" t="s">
+      <c r="P22" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="Q22" s="33" t="s">
+      <c r="Q22" s="24" t="s">
         <v>136</v>
       </c>
       <c r="R22" s="0"/>
+    </row>
+    <row r="23" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="31" t="n">
+        <v>58943</v>
+      </c>
+      <c r="B23" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="F23" s="0"/>
+      <c r="G23" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H23" s="34" t="n">
+        <v>42110</v>
+      </c>
+      <c r="I23" s="34" t="n">
+        <v>42110</v>
+      </c>
+      <c r="J23" s="34" t="n">
+        <v>43936</v>
+      </c>
+      <c r="K23" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="M23" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="N23" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="O23" s="0"/>
+      <c r="P23" s="0"/>
+      <c r="Q23" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="R23" s="38" t="s">
+        <v>171</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Correct return parameter for search_galenic_info
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -20,20 +20,20 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$11635</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$4:$R$11635</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11635</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11634</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11635</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="177">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -539,6 +539,21 @@
 .
 I) et II) et III) corresp.: aminoacida 57.44 g/l, nitrogenia 8 g/l, carbohydrata 144 g/l, materia crassa 40 g/l, natrium 53.6 mmol/l, kalium 37.6 mmol/l, magnesium 4.24 mmol/l, calcium 4.24 mmol/l, zincum 0.032 mmol/l, chloridum 48 mmol/l, phosphas 16 mmol/l, acetas 48 mmol/l, in emulsione recenter mixta 1000 ml.
 Corresp. 4941 kJ pro 1 l.</t>
+  </si>
+  <si>
+    <t>Kefzol 1 g, Injektionsflasche (i.m., i.v.)</t>
+  </si>
+  <si>
+    <t>Teva Pharma AG</t>
+  </si>
+  <si>
+    <t>J01DB04</t>
+  </si>
+  <si>
+    <t>cefazolinum</t>
+  </si>
+  <si>
+    <t>Praeparatio sicca: cefazolinum 1 g ut cefazolinum natricum pro vitro.</t>
   </si>
   <si>
     <t>Apligraf</t>
@@ -888,12 +903,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1410" topLeftCell="A1" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="M23" activeCellId="0" sqref="M23"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="23:23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1969,7 +1984,7 @@
     </row>
     <row r="23" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="31" t="n">
-        <v>58943</v>
+        <v>38210</v>
       </c>
       <c r="B23" s="32" t="n">
         <v>1</v>
@@ -1981,40 +1996,94 @@
         <v>165</v>
       </c>
       <c r="E23" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="F23" s="0"/>
       <c r="G23" s="32" t="s">
-        <v>167</v>
+        <v>56</v>
       </c>
       <c r="H23" s="34" t="n">
-        <v>42110</v>
+        <v>27079</v>
       </c>
       <c r="I23" s="34" t="n">
-        <v>42110</v>
+        <v>27079</v>
       </c>
       <c r="J23" s="34" t="n">
-        <v>43936</v>
+        <v>43434</v>
       </c>
       <c r="K23" s="35" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="L23" s="32" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="M23" s="36" t="s">
-        <v>169</v>
+        <v>99</v>
       </c>
       <c r="N23" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="O23" s="0"/>
-      <c r="P23" s="0"/>
+      <c r="O23" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="P23" s="33" t="s">
+        <v>168</v>
+      </c>
       <c r="Q23" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="R23" s="0"/>
+    </row>
+    <row r="24" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="31" t="n">
+        <v>58943</v>
+      </c>
+      <c r="B24" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="D24" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="R23" s="38" t="s">
+      <c r="E24" s="32" t="s">
         <v>171</v>
+      </c>
+      <c r="F24" s="0"/>
+      <c r="G24" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="H24" s="34" t="n">
+        <v>42110</v>
+      </c>
+      <c r="I24" s="34" t="n">
+        <v>42110</v>
+      </c>
+      <c r="J24" s="34" t="n">
+        <v>43936</v>
+      </c>
+      <c r="K24" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="L24" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="M24" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="N24" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="O24" s="0"/>
+      <c r="P24" s="0"/>
+      <c r="Q24" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="R24" s="38" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Caverjet by eliminatins semantically wrong leading "Solvens:"
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -20,12 +20,13 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$11635</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$4:$R$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$4:$R$11635</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11635</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11635</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="182">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -579,6 +580,21 @@
   <si>
     <t>Behandlung von chronischen venösen Beinulzera sowie von diabetischen Fussulzera 
 Behandlung von Muco-Gingivalen Läsionen (Anwendung nur nach  Herstellung  mit Rinderhypophysenextrakt aus einem Land Kategorie A)</t>
+  </si>
+  <si>
+    <t>Caverject DC 20, Injektionspräparat</t>
+  </si>
+  <si>
+    <t>Pfizer AG</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Spritze(n)</t>
+  </si>
+  <si>
+    <t>Solvens: alprostadilum 20 µg, alfadexum, lactosum anhydricum, natrii citras dihydricus, conserv.: alcohol benzylicus 4.45 mg, aqua ad iniectabilia q.s. ad solutionem pro 0.5 ml in solutione recenter reconstituta.</t>
   </si>
 </sst>
 </file>
@@ -687,7 +703,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -810,38 +826,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -861,15 +845,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>216000</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1127880</xdr:colOff>
+      <xdr:colOff>1154520</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>540360</xdr:rowOff>
+      <xdr:rowOff>540000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -882,8 +866,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="216000" y="0"/>
-          <a:ext cx="1778400" cy="540360"/>
+          <a:off x="243000" y="0"/>
+          <a:ext cx="1778040" cy="540000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -903,12 +887,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R24"/>
+  <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1410" topLeftCell="A1" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="1245" topLeftCell="A1" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="23:23"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="5:23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1982,108 +1966,159 @@
       </c>
       <c r="R22" s="0"/>
     </row>
-    <row r="23" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="31" t="n">
+    <row r="23" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="23" t="n">
         <v>38210</v>
       </c>
-      <c r="B23" s="32" t="n">
+      <c r="B23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C23" s="33" t="s">
+      <c r="C23" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E23" s="32" t="s">
+      <c r="E23" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F23" s="32" t="s">
+      <c r="F23" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G23" s="32" t="s">
+      <c r="G23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H23" s="34" t="n">
+      <c r="H23" s="25" t="n">
         <v>27079</v>
       </c>
-      <c r="I23" s="34" t="n">
+      <c r="I23" s="25" t="n">
         <v>27079</v>
       </c>
-      <c r="J23" s="34" t="n">
+      <c r="J23" s="25" t="n">
         <v>43434</v>
       </c>
-      <c r="K23" s="35" t="n">
+      <c r="K23" s="26" t="n">
         <v>25</v>
       </c>
-      <c r="L23" s="32" t="s">
+      <c r="L23" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="M23" s="36" t="s">
+      <c r="M23" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="N23" s="37" t="s">
+      <c r="N23" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="O23" s="33" t="s">
+      <c r="O23" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="P23" s="33" t="s">
+      <c r="P23" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="Q23" s="33" t="s">
+      <c r="Q23" s="24" t="s">
         <v>103</v>
       </c>
       <c r="R23" s="0"/>
     </row>
-    <row r="24" s="33" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="31" t="n">
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="23" t="n">
         <v>58943</v>
       </c>
-      <c r="B24" s="32" t="n">
+      <c r="B24" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="D24" s="32" t="s">
+      <c r="D24" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="1" t="s">
         <v>171</v>
       </c>
       <c r="F24" s="0"/>
-      <c r="G24" s="32" t="s">
+      <c r="G24" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="H24" s="34" t="n">
+      <c r="H24" s="25" t="n">
         <v>42110</v>
       </c>
-      <c r="I24" s="34" t="n">
+      <c r="I24" s="25" t="n">
         <v>42110</v>
       </c>
-      <c r="J24" s="34" t="n">
+      <c r="J24" s="25" t="n">
         <v>43936</v>
       </c>
-      <c r="K24" s="35" t="n">
+      <c r="K24" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="L24" s="32" t="s">
+      <c r="L24" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="M24" s="36" t="s">
+      <c r="M24" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="N24" s="37" t="s">
+      <c r="N24" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="O24" s="0"/>
-      <c r="P24" s="0"/>
-      <c r="Q24" s="33" t="s">
+      <c r="Q24" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="R24" s="38" t="s">
+      <c r="R24" s="29" t="s">
         <v>176</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="23" t="n">
+        <v>55674</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25" s="25" t="n">
+        <v>37321</v>
+      </c>
+      <c r="I25" s="25" t="n">
+        <v>37321</v>
+      </c>
+      <c r="J25" s="25" t="n">
+        <v>42798</v>
+      </c>
+      <c r="K25" s="26" t="n">
+        <v>7</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="O25" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="P25" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q25" s="0" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Consider changes in ATC-codes by EPha
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -21,6 +21,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$11635</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$4:$R$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$4:$R$11635</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="191">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -595,6 +596,33 @@
   </si>
   <si>
     <t>Solvens: alprostadilum 20 µg, alfadexum, lactosum anhydricum, natrii citras dihydricus, conserv.: alcohol benzylicus 4.45 mg, aqua ad iniectabilia q.s. ad solutionem pro 0.5 ml in solutione recenter reconstituta.</t>
+  </si>
+  <si>
+    <t>Hirudoid, Creme</t>
+  </si>
+  <si>
+    <t>Medinova AG</t>
+  </si>
+  <si>
+    <t>02.08.2.</t>
+  </si>
+  <si>
+    <t>C05BA</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>heparinoidum (chondroitini polysulfas)</t>
+  </si>
+  <si>
+    <t>heparinoidum (chondroitini polysulfas) 3 mg alcoholes adipis lanae, aromatica, conserv.: E 218, E 216, excipiens ad unguentum pro 1 g.</t>
+  </si>
+  <si>
+    <t>Venenmittel für den äusserlichen Gebrauch</t>
   </si>
 </sst>
 </file>
@@ -845,15 +873,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>270000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1154520</xdr:colOff>
+      <xdr:colOff>1181160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>540000</xdr:rowOff>
+      <xdr:rowOff>539640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -866,8 +894,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="243000" y="0"/>
-          <a:ext cx="1778040" cy="540000"/>
+          <a:off x="270000" y="0"/>
+          <a:ext cx="1777680" cy="539640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -887,12 +915,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1245" topLeftCell="A1" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="1095" topLeftCell="A1" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="5:23"/>
+      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="26:26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1966,7 +1994,7 @@
       </c>
       <c r="R22" s="0"/>
     </row>
-    <row r="23" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="23" t="n">
         <v>38210</v>
       </c>
@@ -2018,7 +2046,6 @@
       <c r="Q23" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="R23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="23" t="n">
@@ -2119,6 +2146,59 @@
       </c>
       <c r="Q25" s="0" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="23" t="n">
+        <v>16105</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26" s="25" t="n">
+        <v>18872</v>
+      </c>
+      <c r="I26" s="25" t="n">
+        <v>18872</v>
+      </c>
+      <c r="J26" s="25" t="n">
+        <v>43162</v>
+      </c>
+      <c r="K26" s="26" t="n">
+        <v>58</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O26" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="P26" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q26" s="0" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Give substances for lines starting with Solvens
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package-galenic.xlsx
+++ b/spec/data/swissmedic_package-galenic.xlsx
@@ -23,11 +23,11 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$11635</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$4:$R$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$4:$R$11635</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11635</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$4:$R$11635</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="197">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -623,6 +623,25 @@
   </si>
   <si>
     <t>Venenmittel für den äusserlichen Gebrauch</t>
+  </si>
+  <si>
+    <t>Solu-Cortef 100 mg, Injektions-/Infusionspräparat</t>
+  </si>
+  <si>
+    <t>07.07.21</t>
+  </si>
+  <si>
+    <t>H02AB09</t>
+  </si>
+  <si>
+    <t>hydrocortisonum</t>
+  </si>
+  <si>
+    <t>Praeparatio cryodesiccata: hydrocortisonum 100 mg ut hydrocortisoni-21 succinas natricus, natrii dihydrogenophosphas monohydricus, dinatrii phosphas anhydricus pro vitro.
+Solvens: conserv.: alcohol benzylicus 18 mg, aqua ad iniectabilia q.s. ad solutionem pro 2 ml.</t>
+  </si>
+  <si>
+    <t>Glucocorticoid-Therapie</t>
   </si>
 </sst>
 </file>
@@ -915,12 +934,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:R65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1095" topLeftCell="A1" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="26:26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1095" topLeftCell="A1" activePane="topLeft" state="split"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="5:26"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2201,6 +2220,60 @@
         <v>190</v>
       </c>
     </row>
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="23" t="n">
+        <v>23533</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H27" s="25" t="n">
+        <v>21025</v>
+      </c>
+      <c r="I27" s="25" t="n">
+        <v>21025</v>
+      </c>
+      <c r="J27" s="25" t="n">
+        <v>43800</v>
+      </c>
+      <c r="K27" s="26" t="n">
+        <v>30</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O27" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="P27" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q27" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:M2"/>

</xml_diff>